<commit_message>
Added look ahead and implemented a future co2 price
</commit_message>
<xml_diff>
--- a/resources/configurations/Coupling Config.xlsx
+++ b/resources/configurations/Coupling Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753928F0-407E-43FA-8A10-33B8386774B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEEC63C-2211-4AA5-9E5A-F5231D647AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5670" windowWidth="28800" windowHeight="15435" xr2:uid="{0615D95F-70E0-4B73-ABCC-D3A4B52943C0}"/>
+    <workbookView xWindow="1305" yWindow="3855" windowWidth="28800" windowHeight="15435" xr2:uid="{0615D95F-70E0-4B73-ABCC-D3A4B52943C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Coupling Parameters" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={76D435CB-A853-44AC-A58C-CA521982DF1D}</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{76D435CB-A853-44AC-A58C-CA521982DF1D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Be sure that there is data ready until 'End Year' + 'Look Ahead'</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Start Year</t>
   </si>
@@ -44,18 +62,27 @@
   <si>
     <t>End Year</t>
   </si>
+  <si>
+    <t>Look Ahead</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,6 +122,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jim Hommes" id="{73E6E149-D2EF-4AD4-AF01-C17FEC0FA65E}" userId="f8e3335dd711e3d1" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,12 +425,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B4" dT="2021-07-21T19:07:16.82" personId="{73E6E149-D2EF-4AD4-AF01-C17FEC0FA65E}" id="{76D435CB-A853-44AC-A58C-CA521982DF1D}">
+    <text>Be sure that there is data ready until 'End Year' + 'Look Ahead'</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C92435D-079F-4D06-9F35-FF543A265F4C}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C92435D-079F-4D06-9F35-FF543A265F4C}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,10 +467,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2030</v>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>